<commit_message>
correct typo orderedNumber to orderNumber
</commit_message>
<xml_diff>
--- a/items-creator/examples/excel.xlsx
+++ b/items-creator/examples/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuel/EPFL/Biot/tools/items-creator/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F52D281-BBFF-7745-B37F-744DA9524963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ABBDEA-791E-5642-ACE5-03EDBD10C508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="6180" windowWidth="33600" windowHeight="20500" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{345AA04F-B42B-5143-968F-05FF6E902C33}"/>
   </bookViews>
   <sheets>
     <sheet name="excel" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>previousOwner</t>
   </si>
   <si>
-    <t>orderedNumber</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>this is a comment</t>
+  </si>
+  <si>
+    <t>orderNumber</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,81 +653,81 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="I2">
         <v>999.9</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="P2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>